<commit_message>
Arreglats guardar tots els resultats al Excel
</commit_message>
<xml_diff>
--- a/TFG/res/pacientData/1006/Resultats_REM-G1006.xlsx
+++ b/TFG/res/pacientData/1006/Resultats_REM-G1006.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="644">
   <si>
     <t>ID</t>
   </si>
@@ -743,6 +743,18 @@
     <t>FV - Animals_T1</t>
   </si>
   <si>
+    <t>Fluencia verbal NSSA - P_T1</t>
+  </si>
+  <si>
+    <t>FV NSSA - M_T1</t>
+  </si>
+  <si>
+    <t>FV NSSA - R_T1</t>
+  </si>
+  <si>
+    <t>FV NSSA - Animals_T1</t>
+  </si>
+  <si>
     <t>EPT_T1</t>
   </si>
   <si>
@@ -1112,6 +1124,18 @@
     <t>FV - Animals_T2</t>
   </si>
   <si>
+    <t>Fluencia verbal NSSA - P_T2</t>
+  </si>
+  <si>
+    <t>FV NSSA - M_T2</t>
+  </si>
+  <si>
+    <t>FV NSSA - R_T2</t>
+  </si>
+  <si>
+    <t>FV NSSA - Animals_T2</t>
+  </si>
+  <si>
     <t>EPT_T2</t>
   </si>
   <si>
@@ -1481,6 +1505,18 @@
     <t>FV - Animals_T3</t>
   </si>
   <si>
+    <t>Fluencia verbal NSSA - P_T3</t>
+  </si>
+  <si>
+    <t>FV NSSA - M_T3</t>
+  </si>
+  <si>
+    <t>FV NSSA - R_T3</t>
+  </si>
+  <si>
+    <t>FV NSSA - Animals_T3</t>
+  </si>
+  <si>
     <t>EPT_T3</t>
   </si>
   <si>
@@ -1550,111 +1586,114 @@
     <t>Estudis primaris complets</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Vidu</t>
+  </si>
+  <si>
+    <t>Administrativa</t>
+  </si>
+  <si>
+    <t>Personal suport administratiu</t>
+  </si>
+  <si>
+    <t>En actiu</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No </t>
+  </si>
+  <si>
+    <t>Mai</t>
+  </si>
+  <si>
+    <t>Malaltia d'ALzheimer</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>01/06/2017</t>
+  </si>
+  <si>
+    <t>10/06/2015</t>
+  </si>
+  <si>
+    <t>02/06/2017</t>
+  </si>
+  <si>
+    <t>Sinemet</t>
+  </si>
+  <si>
+    <t>Metformina</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Resultats normals</t>
+  </si>
+  <si>
+    <t>Anormal NCS</t>
+  </si>
+  <si>
+    <t>No realitzat</t>
+  </si>
+  <si>
+    <t>1,6 (Deteriorament moderat)</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Rang mig-baix</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puntuació total de 30, no comet errors. </t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>41-59</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
     <t>8</t>
   </si>
   <si>
-    <t>Vidu</t>
-  </si>
-  <si>
-    <t>Administrativa</t>
-  </si>
-  <si>
-    <t>Personal suport administratiu</t>
-  </si>
-  <si>
-    <t>En actiu</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Sí</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No </t>
-  </si>
-  <si>
-    <t>Mai</t>
-  </si>
-  <si>
-    <t>Malaltia d'ALzheimer</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Si</t>
-  </si>
-  <si>
-    <t>01/06/2017</t>
-  </si>
-  <si>
-    <t>10/06/2015</t>
-  </si>
-  <si>
-    <t>02/06/2017</t>
-  </si>
-  <si>
-    <t>Sinemet</t>
-  </si>
-  <si>
-    <t>Metformina</t>
-  </si>
-  <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>Resultats normals</t>
-  </si>
-  <si>
-    <t>Anormal NCS</t>
-  </si>
-  <si>
-    <t>No realitzat</t>
-  </si>
-  <si>
-    <t>1,6 (Deteriorament moderat)</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Rang mig-baix</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Puntuació total de 30, no comet errors. </t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>41-59</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>60-71</t>
   </si>
   <si>
@@ -1700,9 +1739,6 @@
     <t>133615</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>268804</t>
   </si>
   <si>
@@ -1799,6 +1835,9 @@
     <t>00:01.68</t>
   </si>
   <si>
+    <t>999</t>
+  </si>
+  <si>
     <t>25</t>
   </si>
   <si>
@@ -1850,6 +1889,9 @@
     <t>00:01.06</t>
   </si>
   <si>
+    <t>8888</t>
+  </si>
+  <si>
     <t>28</t>
   </si>
   <si>
@@ -1881,6 +1923,9 @@
   </si>
   <si>
     <t>00:02.52</t>
+  </si>
+  <si>
+    <t>7777</t>
   </si>
   <si>
     <t>18.75</t>
@@ -2911,19 +2956,19 @@
         <v>242</v>
       </c>
       <c r="LI1" t="s">
-        <v>137</v>
+        <v>243</v>
       </c>
       <c r="LJ1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="LK1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="LL1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="LM1" t="s">
-        <v>246</v>
+        <v>137</v>
       </c>
       <c r="LN1" t="s">
         <v>247</v>
@@ -2953,46 +2998,46 @@
         <v>255</v>
       </c>
       <c r="LW1" t="s">
-        <v>137</v>
+        <v>256</v>
       </c>
       <c r="LX1" t="s">
+        <v>257</v>
+      </c>
+      <c r="LY1" t="s">
+        <v>258</v>
+      </c>
+      <c r="LZ1" t="s">
+        <v>259</v>
+      </c>
+      <c r="MA1" t="s">
+        <v>137</v>
+      </c>
+      <c r="MB1" t="s">
+        <v>260</v>
+      </c>
+      <c r="MC1" t="s">
+        <v>261</v>
+      </c>
+      <c r="MD1" t="s">
+        <v>253</v>
+      </c>
+      <c r="ME1" t="s">
+        <v>254</v>
+      </c>
+      <c r="MF1" t="s">
+        <v>262</v>
+      </c>
+      <c r="MG1" t="s">
+        <v>263</v>
+      </c>
+      <c r="MH1" t="s">
         <v>256</v>
       </c>
-      <c r="LY1" t="s">
-        <v>257</v>
-      </c>
-      <c r="LZ1" t="s">
-        <v>249</v>
-      </c>
-      <c r="MA1" t="s">
-        <v>250</v>
-      </c>
-      <c r="MB1" t="s">
-        <v>258</v>
-      </c>
-      <c r="MC1" t="s">
-        <v>259</v>
-      </c>
-      <c r="MD1" t="s">
-        <v>252</v>
-      </c>
-      <c r="ME1" t="s">
-        <v>260</v>
-      </c>
-      <c r="MF1" t="s">
-        <v>137</v>
-      </c>
-      <c r="MG1" t="s">
-        <v>261</v>
-      </c>
-      <c r="MH1" t="s">
-        <v>262</v>
-      </c>
       <c r="MI1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="MJ1" t="s">
-        <v>264</v>
+        <v>137</v>
       </c>
       <c r="MK1" t="s">
         <v>265</v>
@@ -3298,31 +3343,31 @@
         <v>365</v>
       </c>
       <c r="QH1" t="s">
-        <v>137</v>
+        <v>366</v>
       </c>
       <c r="QI1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="QJ1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="QK1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="QL1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="QM1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="QN1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="QO1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="QP1" t="s">
-        <v>373</v>
+        <v>137</v>
       </c>
       <c r="QQ1" t="s">
         <v>374</v>
@@ -3340,58 +3385,58 @@
         <v>378</v>
       </c>
       <c r="QV1" t="s">
-        <v>137</v>
+        <v>379</v>
       </c>
       <c r="QW1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="QX1" t="s">
+        <v>381</v>
+      </c>
+      <c r="QY1" t="s">
+        <v>382</v>
+      </c>
+      <c r="QZ1" t="s">
+        <v>383</v>
+      </c>
+      <c r="RA1" t="s">
+        <v>384</v>
+      </c>
+      <c r="RB1" t="s">
+        <v>385</v>
+      </c>
+      <c r="RC1" t="s">
+        <v>386</v>
+      </c>
+      <c r="RD1" t="s">
+        <v>137</v>
+      </c>
+      <c r="RE1" t="s">
+        <v>387</v>
+      </c>
+      <c r="RF1" t="s">
+        <v>388</v>
+      </c>
+      <c r="RG1" t="s">
         <v>380</v>
       </c>
-      <c r="QY1" t="s">
-        <v>372</v>
-      </c>
-      <c r="QZ1" t="s">
-        <v>373</v>
-      </c>
-      <c r="RA1" t="s">
+      <c r="RH1" t="s">
         <v>381</v>
       </c>
-      <c r="RB1" t="s">
-        <v>382</v>
-      </c>
-      <c r="RC1" t="s">
-        <v>375</v>
-      </c>
-      <c r="RD1" t="s">
+      <c r="RI1" t="s">
+        <v>389</v>
+      </c>
+      <c r="RJ1" t="s">
+        <v>390</v>
+      </c>
+      <c r="RK1" t="s">
         <v>383</v>
       </c>
-      <c r="RE1" t="s">
-        <v>137</v>
-      </c>
-      <c r="RF1" t="s">
-        <v>384</v>
-      </c>
-      <c r="RG1" t="s">
-        <v>385</v>
-      </c>
-      <c r="RH1" t="s">
-        <v>386</v>
-      </c>
-      <c r="RI1" t="s">
-        <v>387</v>
-      </c>
-      <c r="RJ1" t="s">
-        <v>388</v>
-      </c>
-      <c r="RK1" t="s">
-        <v>389</v>
-      </c>
       <c r="RL1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="RM1" t="s">
-        <v>391</v>
+        <v>137</v>
       </c>
       <c r="RN1" t="s">
         <v>392</v>
@@ -3685,1878 +3730,1950 @@
         <v>488</v>
       </c>
       <c r="VG1" t="s">
-        <v>137</v>
+        <v>489</v>
       </c>
       <c r="VH1" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="VI1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="VJ1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="VK1" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="VL1" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="VM1" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="VN1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="VO1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="VP1" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="VQ1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="VR1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="VS1" t="s">
-        <v>500</v>
+        <v>137</v>
       </c>
       <c r="VT1" t="s">
         <v>501</v>
       </c>
       <c r="VU1" t="s">
-        <v>137</v>
+        <v>502</v>
       </c>
       <c r="VV1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="VW1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="VX1" t="s">
-        <v>495</v>
+        <v>505</v>
       </c>
       <c r="VY1" t="s">
-        <v>496</v>
+        <v>506</v>
       </c>
       <c r="VZ1" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="WA1" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="WB1" t="s">
-        <v>498</v>
+        <v>509</v>
       </c>
       <c r="WC1" t="s">
-        <v>506</v>
+        <v>510</v>
+      </c>
+      <c r="WD1" t="s">
+        <v>511</v>
+      </c>
+      <c r="WE1" t="s">
+        <v>512</v>
+      </c>
+      <c r="WF1" t="s">
+        <v>513</v>
+      </c>
+      <c r="WG1" t="s">
+        <v>137</v>
+      </c>
+      <c r="WH1" t="s">
+        <v>514</v>
+      </c>
+      <c r="WI1" t="s">
+        <v>515</v>
+      </c>
+      <c r="WJ1" t="s">
+        <v>507</v>
+      </c>
+      <c r="WK1" t="s">
+        <v>508</v>
+      </c>
+      <c r="WL1" t="s">
+        <v>516</v>
+      </c>
+      <c r="WM1" t="s">
+        <v>517</v>
+      </c>
+      <c r="WN1" t="s">
+        <v>510</v>
+      </c>
+      <c r="WO1" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>507</v>
+        <v>519</v>
       </c>
       <c r="B2" t="s">
-        <v>507</v>
+        <v>519</v>
       </c>
       <c r="C2" t="s">
-        <v>508</v>
+        <v>520</v>
       </c>
       <c r="D2" t="s">
-        <v>509</v>
+        <v>521</v>
       </c>
       <c r="E2" t="s">
-        <v>510</v>
+        <v>522</v>
       </c>
       <c r="F2" t="s">
-        <v>511</v>
+        <v>523</v>
       </c>
       <c r="G2" t="s">
-        <v>512</v>
+        <v>524</v>
       </c>
       <c r="H2" t="s">
-        <v>513</v>
+        <v>525</v>
       </c>
       <c r="I2" t="s">
-        <v>514</v>
+        <v>526</v>
       </c>
       <c r="J2" t="s">
-        <v>515</v>
+        <v>527</v>
       </c>
       <c r="K2" t="s">
-        <v>516</v>
+        <v>528</v>
       </c>
       <c r="L2" t="s">
-        <v>517</v>
+        <v>529</v>
       </c>
       <c r="M2" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="N2" t="s">
-        <v>517</v>
+        <v>529</v>
       </c>
       <c r="O2" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="P2" t="s">
-        <v>520</v>
+        <v>532</v>
       </c>
       <c r="Q2" t="s">
-        <v>521</v>
+        <v>533</v>
       </c>
       <c r="R2" t="s">
-        <v>521</v>
+        <v>533</v>
       </c>
       <c r="S2" t="s">
-        <v>522</v>
+        <v>534</v>
       </c>
       <c r="T2" t="s">
-        <v>522</v>
+        <v>534</v>
       </c>
       <c r="U2" t="s">
-        <v>522</v>
+        <v>534</v>
       </c>
       <c r="V2" t="s">
-        <v>523</v>
+        <v>535</v>
       </c>
       <c r="W2" t="s">
+        <v>536</v>
+      </c>
+      <c r="X2" t="s">
+        <v>533</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>533</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>533</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>533</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>535</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>537</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>533</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>538</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>539</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>534</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>533</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>533</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>533</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>530</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>540</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>533</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>533</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>533</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>533</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>533</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>533</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>533</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>533</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>533</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>530</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>541</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>533</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>533</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>533</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>533</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>530</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>542</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>533</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>533</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>533</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>533</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>533</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>533</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>533</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>533</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>533</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>533</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>533</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>533</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>533</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>533</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>533</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>533</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>533</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>533</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>533</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>533</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>533</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>533</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>533</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>533</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DU2" t="s">
+        <v>543</v>
+      </c>
+      <c r="DV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>544</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="ER2" t="s">
+        <v>137</v>
+      </c>
+      <c r="ES2" t="s">
+        <v>137</v>
+      </c>
+      <c r="ET2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EU2" t="s">
+        <v>545</v>
+      </c>
+      <c r="EV2" t="s">
+        <v>546</v>
+      </c>
+      <c r="EW2" t="s">
+        <v>540</v>
+      </c>
+      <c r="EX2" t="s">
+        <v>547</v>
+      </c>
+      <c r="EY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="EZ2" t="s">
+        <v>540</v>
+      </c>
+      <c r="FA2" t="s">
+        <v>545</v>
+      </c>
+      <c r="FB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FC2" t="s">
+        <v>540</v>
+      </c>
+      <c r="FD2" t="s">
+        <v>548</v>
+      </c>
+      <c r="FE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FG2" t="s">
+        <v>548</v>
+      </c>
+      <c r="FH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FJ2" t="s">
+        <v>548</v>
+      </c>
+      <c r="FK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FM2" t="s">
+        <v>548</v>
+      </c>
+      <c r="FN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FP2" t="s">
+        <v>548</v>
+      </c>
+      <c r="FQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FS2" t="s">
+        <v>548</v>
+      </c>
+      <c r="FT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FV2" t="s">
+        <v>548</v>
+      </c>
+      <c r="FW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="FY2" t="s">
+        <v>548</v>
+      </c>
+      <c r="FZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GB2" t="s">
+        <v>548</v>
+      </c>
+      <c r="GC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GE2" t="s">
+        <v>548</v>
+      </c>
+      <c r="GF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GH2" t="s">
+        <v>548</v>
+      </c>
+      <c r="GI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GK2" t="s">
+        <v>548</v>
+      </c>
+      <c r="GL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GN2" t="s">
+        <v>548</v>
+      </c>
+      <c r="GO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GQ2" t="s">
+        <v>548</v>
+      </c>
+      <c r="GR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GT2" t="s">
+        <v>548</v>
+      </c>
+      <c r="GU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GW2" t="s">
+        <v>548</v>
+      </c>
+      <c r="GX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="GZ2" t="s">
+        <v>549</v>
+      </c>
+      <c r="HA2" t="s">
+        <v>550</v>
+      </c>
+      <c r="HB2" t="s">
+        <v>551</v>
+      </c>
+      <c r="HC2" t="s">
+        <v>552</v>
+      </c>
+      <c r="HD2" t="s">
+        <v>553</v>
+      </c>
+      <c r="HE2" t="s">
+        <v>554</v>
+      </c>
+      <c r="HF2" t="s">
+        <v>555</v>
+      </c>
+      <c r="HG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HH2" t="s">
+        <v>556</v>
+      </c>
+      <c r="HI2" t="s">
+        <v>550</v>
+      </c>
+      <c r="HJ2" t="s">
+        <v>557</v>
+      </c>
+      <c r="HK2" t="s">
+        <v>558</v>
+      </c>
+      <c r="HL2" t="s">
+        <v>529</v>
+      </c>
+      <c r="HM2" t="s">
+        <v>559</v>
+      </c>
+      <c r="HN2" t="s">
+        <v>560</v>
+      </c>
+      <c r="HO2" t="s">
+        <v>561</v>
+      </c>
+      <c r="HP2" t="s">
+        <v>562</v>
+      </c>
+      <c r="HQ2" t="s">
+        <v>563</v>
+      </c>
+      <c r="HR2" t="s">
+        <v>564</v>
+      </c>
+      <c r="HS2" t="s">
+        <v>565</v>
+      </c>
+      <c r="HT2" t="s">
+        <v>538</v>
+      </c>
+      <c r="HU2" t="s">
+        <v>534</v>
+      </c>
+      <c r="HV2" t="s">
+        <v>566</v>
+      </c>
+      <c r="HW2" t="s">
+        <v>567</v>
+      </c>
+      <c r="HX2" t="s">
+        <v>568</v>
+      </c>
+      <c r="HY2" t="s">
+        <v>556</v>
+      </c>
+      <c r="HZ2" t="s">
+        <v>534</v>
+      </c>
+      <c r="IA2" t="s">
+        <v>566</v>
+      </c>
+      <c r="IB2" t="s">
+        <v>569</v>
+      </c>
+      <c r="IC2" t="s">
+        <v>570</v>
+      </c>
+      <c r="ID2" t="s">
+        <v>550</v>
+      </c>
+      <c r="IE2" t="s">
+        <v>534</v>
+      </c>
+      <c r="IF2" t="s">
+        <v>566</v>
+      </c>
+      <c r="IG2" t="s">
+        <v>571</v>
+      </c>
+      <c r="IH2" t="s">
+        <v>538</v>
+      </c>
+      <c r="II2" t="s">
+        <v>572</v>
+      </c>
+      <c r="IJ2" t="s">
+        <v>573</v>
+      </c>
+      <c r="IK2" t="s">
+        <v>574</v>
+      </c>
+      <c r="IL2" t="s">
+        <v>554</v>
+      </c>
+      <c r="IM2" t="s">
         <v>524</v>
       </c>
-      <c r="X2" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>521</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>521</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>521</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>523</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>525</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>521</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>526</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>527</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>522</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>521</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>521</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>521</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>518</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>528</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>521</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>137</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>521</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>137</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>521</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>137</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>521</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>137</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>521</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>137</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>521</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>137</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>521</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>521</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>521</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>518</v>
-      </c>
-      <c r="BF2" t="s">
+      <c r="IN2" t="s">
+        <v>575</v>
+      </c>
+      <c r="IO2" t="s">
+        <v>576</v>
+      </c>
+      <c r="IP2" t="s">
+        <v>577</v>
+      </c>
+      <c r="IQ2" t="s">
+        <v>578</v>
+      </c>
+      <c r="IR2" t="s">
+        <v>579</v>
+      </c>
+      <c r="IS2" t="s">
+        <v>580</v>
+      </c>
+      <c r="IT2" t="s">
+        <v>581</v>
+      </c>
+      <c r="IU2" t="s">
+        <v>582</v>
+      </c>
+      <c r="IV2" t="s">
+        <v>583</v>
+      </c>
+      <c r="IW2" t="s">
+        <v>558</v>
+      </c>
+      <c r="IX2" t="s">
+        <v>584</v>
+      </c>
+      <c r="IY2" t="s">
+        <v>585</v>
+      </c>
+      <c r="IZ2" t="s">
+        <v>586</v>
+      </c>
+      <c r="JA2" t="s">
+        <v>583</v>
+      </c>
+      <c r="JB2" t="s">
+        <v>587</v>
+      </c>
+      <c r="JC2" t="s">
+        <v>588</v>
+      </c>
+      <c r="JD2" t="s">
+        <v>589</v>
+      </c>
+      <c r="JE2" t="s">
+        <v>590</v>
+      </c>
+      <c r="JF2" t="s">
+        <v>556</v>
+      </c>
+      <c r="JG2" t="s">
+        <v>538</v>
+      </c>
+      <c r="JH2" t="s">
+        <v>568</v>
+      </c>
+      <c r="JI2" t="s">
+        <v>591</v>
+      </c>
+      <c r="JJ2" t="s">
+        <v>592</v>
+      </c>
+      <c r="JK2" t="s">
+        <v>593</v>
+      </c>
+      <c r="JL2" t="s">
+        <v>594</v>
+      </c>
+      <c r="JM2" t="s">
+        <v>531</v>
+      </c>
+      <c r="JN2" t="s">
+        <v>534</v>
+      </c>
+      <c r="JO2" t="s">
+        <v>595</v>
+      </c>
+      <c r="JP2" t="s">
+        <v>596</v>
+      </c>
+      <c r="JQ2" t="s">
+        <v>524</v>
+      </c>
+      <c r="JR2" t="s">
+        <v>597</v>
+      </c>
+      <c r="JS2" t="s">
+        <v>597</v>
+      </c>
+      <c r="JT2" t="s">
+        <v>598</v>
+      </c>
+      <c r="JU2" t="s">
+        <v>534</v>
+      </c>
+      <c r="JV2" t="s">
+        <v>598</v>
+      </c>
+      <c r="JW2" t="s">
+        <v>534</v>
+      </c>
+      <c r="JX2" t="s">
+        <v>598</v>
+      </c>
+      <c r="JY2" t="s">
+        <v>534</v>
+      </c>
+      <c r="JZ2" t="s">
+        <v>598</v>
+      </c>
+      <c r="KA2" t="s">
+        <v>559</v>
+      </c>
+      <c r="KB2" t="s">
+        <v>597</v>
+      </c>
+      <c r="KC2" t="s">
+        <v>597</v>
+      </c>
+      <c r="KD2" t="s">
+        <v>598</v>
+      </c>
+      <c r="KE2" t="s">
+        <v>534</v>
+      </c>
+      <c r="KF2" t="s">
+        <v>598</v>
+      </c>
+      <c r="KG2" t="s">
+        <v>534</v>
+      </c>
+      <c r="KH2" t="s">
+        <v>598</v>
+      </c>
+      <c r="KI2" t="s">
+        <v>534</v>
+      </c>
+      <c r="KJ2" t="s">
+        <v>598</v>
+      </c>
+      <c r="KK2" t="s">
+        <v>599</v>
+      </c>
+      <c r="KL2" t="s">
+        <v>598</v>
+      </c>
+      <c r="KM2" t="s">
+        <v>600</v>
+      </c>
+      <c r="KN2" t="s">
+        <v>538</v>
+      </c>
+      <c r="KO2" t="s">
+        <v>601</v>
+      </c>
+      <c r="KP2" t="s">
+        <v>602</v>
+      </c>
+      <c r="KQ2" t="s">
+        <v>603</v>
+      </c>
+      <c r="KR2" t="s">
         <v>529</v>
       </c>
-      <c r="BG2" t="s">
-        <v>521</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>521</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>521</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>521</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>518</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>530</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>521</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>521</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>521</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>521</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>521</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>521</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>521</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>521</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>521</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>521</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>521</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>521</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>521</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>521</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>521</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>521</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>521</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>521</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>521</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>521</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>521</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>521</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>521</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>521</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DO2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DP2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DQ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DR2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DS2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DT2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DU2" t="s">
+      <c r="KS2" t="s">
+        <v>556</v>
+      </c>
+      <c r="KT2" t="s">
+        <v>556</v>
+      </c>
+      <c r="KU2" t="s">
+        <v>604</v>
+      </c>
+      <c r="KV2" t="s">
+        <v>605</v>
+      </c>
+      <c r="KW2" t="s">
+        <v>550</v>
+      </c>
+      <c r="KX2" t="s">
+        <v>524</v>
+      </c>
+      <c r="KY2" t="s">
+        <v>606</v>
+      </c>
+      <c r="KZ2" t="s">
+        <v>559</v>
+      </c>
+      <c r="LA2" t="s">
+        <v>593</v>
+      </c>
+      <c r="LB2" t="s">
+        <v>524</v>
+      </c>
+      <c r="LC2" t="s">
+        <v>556</v>
+      </c>
+      <c r="LD2" t="s">
+        <v>529</v>
+      </c>
+      <c r="LE2" t="s">
+        <v>558</v>
+      </c>
+      <c r="LF2" t="s">
+        <v>558</v>
+      </c>
+      <c r="LG2" t="s">
+        <v>550</v>
+      </c>
+      <c r="LH2" t="s">
+        <v>566</v>
+      </c>
+      <c r="LI2" t="s">
+        <v>607</v>
+      </c>
+      <c r="LJ2" t="s">
+        <v>607</v>
+      </c>
+      <c r="LK2" t="s">
+        <v>607</v>
+      </c>
+      <c r="LL2" t="s">
+        <v>607</v>
+      </c>
+      <c r="LM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LN2" t="s">
+        <v>550</v>
+      </c>
+      <c r="LO2" t="s">
+        <v>554</v>
+      </c>
+      <c r="LP2" t="s">
+        <v>608</v>
+      </c>
+      <c r="LQ2" t="s">
+        <v>609</v>
+      </c>
+      <c r="LR2" t="s">
+        <v>610</v>
+      </c>
+      <c r="LS2" t="s">
+        <v>611</v>
+      </c>
+      <c r="LT2" t="s">
+        <v>612</v>
+      </c>
+      <c r="LU2" t="s">
+        <v>550</v>
+      </c>
+      <c r="LV2" t="s">
+        <v>571</v>
+      </c>
+      <c r="LW2" t="s">
+        <v>613</v>
+      </c>
+      <c r="LX2" t="s">
+        <v>614</v>
+      </c>
+      <c r="LY2" t="s">
+        <v>554</v>
+      </c>
+      <c r="LZ2" t="s">
+        <v>615</v>
+      </c>
+      <c r="MA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MB2" t="s">
+        <v>594</v>
+      </c>
+      <c r="MC2" t="s">
+        <v>605</v>
+      </c>
+      <c r="MD2" t="s">
+        <v>566</v>
+      </c>
+      <c r="ME2" t="s">
         <v>531</v>
       </c>
-      <c r="DV2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DW2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DX2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DY2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DZ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EA2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EB2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EC2" t="s">
-        <v>137</v>
-      </c>
-      <c r="ED2" t="s">
-        <v>532</v>
-      </c>
-      <c r="EE2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EF2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EG2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EH2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EI2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EJ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EL2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EM2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EN2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EO2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EP2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EQ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="ER2" t="s">
-        <v>137</v>
-      </c>
-      <c r="ES2" t="s">
-        <v>137</v>
-      </c>
-      <c r="ET2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EU2" t="s">
-        <v>533</v>
-      </c>
-      <c r="EV2" t="s">
+      <c r="MF2" t="s">
+        <v>616</v>
+      </c>
+      <c r="MG2" t="s">
+        <v>571</v>
+      </c>
+      <c r="MH2" t="s">
+        <v>617</v>
+      </c>
+      <c r="MI2" t="s">
+        <v>554</v>
+      </c>
+      <c r="MJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MK2" t="s">
+        <v>529</v>
+      </c>
+      <c r="ML2" t="s">
+        <v>524</v>
+      </c>
+      <c r="MM2" t="s">
+        <v>618</v>
+      </c>
+      <c r="MN2" t="s">
+        <v>559</v>
+      </c>
+      <c r="MO2" t="s">
+        <v>529</v>
+      </c>
+      <c r="MP2" t="s">
+        <v>559</v>
+      </c>
+      <c r="MQ2" t="s">
+        <v>560</v>
+      </c>
+      <c r="MR2" t="s">
+        <v>561</v>
+      </c>
+      <c r="MS2" t="s">
+        <v>611</v>
+      </c>
+      <c r="MT2" t="s">
+        <v>558</v>
+      </c>
+      <c r="MU2" t="s">
+        <v>564</v>
+      </c>
+      <c r="MV2" t="s">
+        <v>565</v>
+      </c>
+      <c r="MW2" t="s">
+        <v>538</v>
+      </c>
+      <c r="MX2" t="s">
         <v>534</v>
       </c>
-      <c r="EW2" t="s">
-        <v>528</v>
-      </c>
-      <c r="EX2" t="s">
-        <v>535</v>
-      </c>
-      <c r="EY2" t="s">
-        <v>137</v>
-      </c>
-      <c r="EZ2" t="s">
-        <v>528</v>
-      </c>
-      <c r="FA2" t="s">
-        <v>533</v>
-      </c>
-      <c r="FB2" t="s">
-        <v>137</v>
-      </c>
-      <c r="FC2" t="s">
-        <v>528</v>
-      </c>
-      <c r="FD2" t="s">
-        <v>536</v>
-      </c>
-      <c r="FE2" t="s">
-        <v>137</v>
-      </c>
-      <c r="FF2" t="s">
-        <v>137</v>
-      </c>
-      <c r="FG2" t="s">
-        <v>536</v>
-      </c>
-      <c r="FH2" t="s">
-        <v>137</v>
-      </c>
-      <c r="FI2" t="s">
-        <v>137</v>
-      </c>
-      <c r="FJ2" t="s">
-        <v>536</v>
-      </c>
-      <c r="FK2" t="s">
-        <v>137</v>
-      </c>
-      <c r="FL2" t="s">
-        <v>137</v>
-      </c>
-      <c r="FM2" t="s">
-        <v>536</v>
-      </c>
-      <c r="FN2" t="s">
-        <v>137</v>
-      </c>
-      <c r="FO2" t="s">
-        <v>137</v>
-      </c>
-      <c r="FP2" t="s">
-        <v>536</v>
-      </c>
-      <c r="FQ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="FR2" t="s">
-        <v>137</v>
-      </c>
-      <c r="FS2" t="s">
-        <v>536</v>
-      </c>
-      <c r="FT2" t="s">
-        <v>137</v>
-      </c>
-      <c r="FU2" t="s">
-        <v>137</v>
-      </c>
-      <c r="FV2" t="s">
-        <v>536</v>
-      </c>
-      <c r="FW2" t="s">
-        <v>137</v>
-      </c>
-      <c r="FX2" t="s">
-        <v>137</v>
-      </c>
-      <c r="FY2" t="s">
-        <v>536</v>
-      </c>
-      <c r="FZ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="GA2" t="s">
-        <v>137</v>
-      </c>
-      <c r="GB2" t="s">
-        <v>536</v>
-      </c>
-      <c r="GC2" t="s">
-        <v>137</v>
-      </c>
-      <c r="GD2" t="s">
-        <v>137</v>
-      </c>
-      <c r="GE2" t="s">
-        <v>536</v>
-      </c>
-      <c r="GF2" t="s">
-        <v>137</v>
-      </c>
-      <c r="GG2" t="s">
-        <v>137</v>
-      </c>
-      <c r="GH2" t="s">
-        <v>536</v>
-      </c>
-      <c r="GI2" t="s">
-        <v>137</v>
-      </c>
-      <c r="GJ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="GK2" t="s">
-        <v>536</v>
-      </c>
-      <c r="GL2" t="s">
-        <v>137</v>
-      </c>
-      <c r="GM2" t="s">
-        <v>137</v>
-      </c>
-      <c r="GN2" t="s">
-        <v>536</v>
-      </c>
-      <c r="GO2" t="s">
-        <v>137</v>
-      </c>
-      <c r="GP2" t="s">
-        <v>137</v>
-      </c>
-      <c r="GQ2" t="s">
-        <v>536</v>
-      </c>
-      <c r="GR2" t="s">
-        <v>137</v>
-      </c>
-      <c r="GS2" t="s">
-        <v>137</v>
-      </c>
-      <c r="GT2" t="s">
-        <v>536</v>
-      </c>
-      <c r="GU2" t="s">
-        <v>137</v>
-      </c>
-      <c r="GV2" t="s">
-        <v>137</v>
-      </c>
-      <c r="GW2" t="s">
-        <v>536</v>
-      </c>
-      <c r="GX2" t="s">
-        <v>137</v>
-      </c>
-      <c r="GY2" t="s">
-        <v>137</v>
-      </c>
-      <c r="GZ2" t="s">
-        <v>537</v>
-      </c>
-      <c r="HA2" t="s">
+      <c r="MY2" t="s">
+        <v>566</v>
+      </c>
+      <c r="MZ2" t="s">
+        <v>567</v>
+      </c>
+      <c r="NA2" t="s">
+        <v>568</v>
+      </c>
+      <c r="NB2" t="s">
+        <v>556</v>
+      </c>
+      <c r="NC2" t="s">
+        <v>534</v>
+      </c>
+      <c r="ND2" t="s">
+        <v>566</v>
+      </c>
+      <c r="NE2" t="s">
+        <v>569</v>
+      </c>
+      <c r="NF2" t="s">
+        <v>570</v>
+      </c>
+      <c r="NG2" t="s">
+        <v>550</v>
+      </c>
+      <c r="NH2" t="s">
+        <v>534</v>
+      </c>
+      <c r="NI2" t="s">
+        <v>566</v>
+      </c>
+      <c r="NJ2" t="s">
+        <v>571</v>
+      </c>
+      <c r="NK2" t="s">
         <v>538</v>
       </c>
-      <c r="HB2" t="s">
-        <v>539</v>
-      </c>
-      <c r="HC2" t="s">
-        <v>540</v>
-      </c>
-      <c r="HD2" t="s">
-        <v>541</v>
-      </c>
-      <c r="HE2" t="s">
-        <v>542</v>
-      </c>
-      <c r="HF2" t="s">
-        <v>543</v>
-      </c>
-      <c r="HG2" t="s">
-        <v>137</v>
-      </c>
-      <c r="HH2" t="s">
-        <v>544</v>
-      </c>
-      <c r="HI2" t="s">
+      <c r="NL2" t="s">
+        <v>572</v>
+      </c>
+      <c r="NM2" t="s">
+        <v>573</v>
+      </c>
+      <c r="NN2" t="s">
+        <v>574</v>
+      </c>
+      <c r="NO2" t="s">
+        <v>554</v>
+      </c>
+      <c r="NP2" t="s">
+        <v>524</v>
+      </c>
+      <c r="NQ2" t="s">
+        <v>575</v>
+      </c>
+      <c r="NR2" t="s">
+        <v>576</v>
+      </c>
+      <c r="NS2" t="s">
+        <v>577</v>
+      </c>
+      <c r="NT2" t="s">
+        <v>578</v>
+      </c>
+      <c r="NU2" t="s">
+        <v>579</v>
+      </c>
+      <c r="NV2" t="s">
+        <v>580</v>
+      </c>
+      <c r="NW2" t="s">
+        <v>581</v>
+      </c>
+      <c r="NX2" t="s">
+        <v>582</v>
+      </c>
+      <c r="NY2" t="s">
+        <v>583</v>
+      </c>
+      <c r="NZ2" t="s">
+        <v>558</v>
+      </c>
+      <c r="OA2" t="s">
+        <v>584</v>
+      </c>
+      <c r="OB2" t="s">
+        <v>585</v>
+      </c>
+      <c r="OC2" t="s">
+        <v>586</v>
+      </c>
+      <c r="OD2" t="s">
+        <v>583</v>
+      </c>
+      <c r="OE2" t="s">
+        <v>587</v>
+      </c>
+      <c r="OF2" t="s">
+        <v>588</v>
+      </c>
+      <c r="OG2" t="s">
+        <v>589</v>
+      </c>
+      <c r="OH2" t="s">
+        <v>590</v>
+      </c>
+      <c r="OI2" t="s">
+        <v>556</v>
+      </c>
+      <c r="OJ2" t="s">
         <v>538</v>
       </c>
-      <c r="HJ2" t="s">
-        <v>545</v>
-      </c>
-      <c r="HK2" t="s">
-        <v>546</v>
-      </c>
-      <c r="HL2" t="s">
-        <v>517</v>
-      </c>
-      <c r="HM2" t="s">
-        <v>512</v>
-      </c>
-      <c r="HN2" t="s">
-        <v>547</v>
-      </c>
-      <c r="HO2" t="s">
-        <v>548</v>
-      </c>
-      <c r="HP2" t="s">
-        <v>549</v>
-      </c>
-      <c r="HQ2" t="s">
+      <c r="OK2" t="s">
+        <v>568</v>
+      </c>
+      <c r="OL2" t="s">
+        <v>591</v>
+      </c>
+      <c r="OM2" t="s">
+        <v>611</v>
+      </c>
+      <c r="ON2" t="s">
+        <v>619</v>
+      </c>
+      <c r="OO2" t="s">
+        <v>594</v>
+      </c>
+      <c r="OP2" t="s">
+        <v>558</v>
+      </c>
+      <c r="OQ2" t="s">
+        <v>559</v>
+      </c>
+      <c r="OR2" t="s">
+        <v>618</v>
+      </c>
+      <c r="OS2" t="s">
         <v>550</v>
       </c>
-      <c r="HR2" t="s">
-        <v>551</v>
-      </c>
-      <c r="HS2" t="s">
-        <v>552</v>
-      </c>
-      <c r="HT2" t="s">
-        <v>526</v>
-      </c>
-      <c r="HU2" t="s">
-        <v>522</v>
-      </c>
-      <c r="HV2" t="s">
-        <v>553</v>
-      </c>
-      <c r="HW2" t="s">
+      <c r="OT2" t="s">
+        <v>529</v>
+      </c>
+      <c r="OU2" t="s">
+        <v>597</v>
+      </c>
+      <c r="OV2" t="s">
+        <v>597</v>
+      </c>
+      <c r="OW2" t="s">
+        <v>598</v>
+      </c>
+      <c r="OX2" t="s">
+        <v>534</v>
+      </c>
+      <c r="OY2" t="s">
+        <v>598</v>
+      </c>
+      <c r="OZ2" t="s">
+        <v>534</v>
+      </c>
+      <c r="PA2" t="s">
+        <v>598</v>
+      </c>
+      <c r="PB2" t="s">
+        <v>534</v>
+      </c>
+      <c r="PC2" t="s">
+        <v>598</v>
+      </c>
+      <c r="PD2" t="s">
+        <v>602</v>
+      </c>
+      <c r="PE2" t="s">
+        <v>597</v>
+      </c>
+      <c r="PF2" t="s">
+        <v>597</v>
+      </c>
+      <c r="PG2" t="s">
+        <v>598</v>
+      </c>
+      <c r="PH2" t="s">
+        <v>534</v>
+      </c>
+      <c r="PI2" t="s">
+        <v>598</v>
+      </c>
+      <c r="PJ2" t="s">
+        <v>534</v>
+      </c>
+      <c r="PK2" t="s">
+        <v>598</v>
+      </c>
+      <c r="PL2" t="s">
+        <v>534</v>
+      </c>
+      <c r="PM2" t="s">
+        <v>598</v>
+      </c>
+      <c r="PN2" t="s">
+        <v>620</v>
+      </c>
+      <c r="PO2" t="s">
+        <v>598</v>
+      </c>
+      <c r="PP2" t="s">
+        <v>621</v>
+      </c>
+      <c r="PQ2" t="s">
+        <v>602</v>
+      </c>
+      <c r="PR2" t="s">
+        <v>556</v>
+      </c>
+      <c r="PS2" t="s">
+        <v>529</v>
+      </c>
+      <c r="PT2" t="s">
+        <v>622</v>
+      </c>
+      <c r="PU2" t="s">
+        <v>556</v>
+      </c>
+      <c r="PV2" t="s">
+        <v>524</v>
+      </c>
+      <c r="PW2" t="s">
+        <v>605</v>
+      </c>
+      <c r="PX2" t="s">
+        <v>623</v>
+      </c>
+      <c r="PY2" t="s">
+        <v>556</v>
+      </c>
+      <c r="PZ2" t="s">
+        <v>561</v>
+      </c>
+      <c r="QA2" t="s">
+        <v>529</v>
+      </c>
+      <c r="QB2" t="s">
+        <v>624</v>
+      </c>
+      <c r="QC2" t="s">
+        <v>602</v>
+      </c>
+      <c r="QD2" t="s">
+        <v>550</v>
+      </c>
+      <c r="QE2" t="s">
+        <v>529</v>
+      </c>
+      <c r="QF2" t="s">
+        <v>605</v>
+      </c>
+      <c r="QG2" t="s">
+        <v>538</v>
+      </c>
+      <c r="QH2" t="s">
+        <v>558</v>
+      </c>
+      <c r="QI2" t="s">
+        <v>558</v>
+      </c>
+      <c r="QJ2" t="s">
+        <v>524</v>
+      </c>
+      <c r="QK2" t="s">
+        <v>531</v>
+      </c>
+      <c r="QL2" t="s">
+        <v>625</v>
+      </c>
+      <c r="QM2" t="s">
+        <v>625</v>
+      </c>
+      <c r="QN2" t="s">
+        <v>625</v>
+      </c>
+      <c r="QO2" t="s">
+        <v>625</v>
+      </c>
+      <c r="QP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QQ2" t="s">
+        <v>550</v>
+      </c>
+      <c r="QR2" t="s">
+        <v>583</v>
+      </c>
+      <c r="QS2" t="s">
+        <v>608</v>
+      </c>
+      <c r="QT2" t="s">
+        <v>609</v>
+      </c>
+      <c r="QU2" t="s">
+        <v>610</v>
+      </c>
+      <c r="QV2" t="s">
+        <v>626</v>
+      </c>
+      <c r="QW2" t="s">
+        <v>559</v>
+      </c>
+      <c r="QX2" t="s">
+        <v>559</v>
+      </c>
+      <c r="QY2" t="s">
+        <v>571</v>
+      </c>
+      <c r="QZ2" t="s">
+        <v>611</v>
+      </c>
+      <c r="RA2" t="s">
+        <v>608</v>
+      </c>
+      <c r="RB2" t="s">
+        <v>601</v>
+      </c>
+      <c r="RC2" t="s">
+        <v>627</v>
+      </c>
+      <c r="RD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RE2" t="s">
+        <v>594</v>
+      </c>
+      <c r="RF2" t="s">
+        <v>534</v>
+      </c>
+      <c r="RG2" t="s">
+        <v>605</v>
+      </c>
+      <c r="RH2" t="s">
+        <v>558</v>
+      </c>
+      <c r="RI2" t="s">
+        <v>628</v>
+      </c>
+      <c r="RJ2" t="s">
+        <v>629</v>
+      </c>
+      <c r="RK2" t="s">
+        <v>583</v>
+      </c>
+      <c r="RL2" t="s">
+        <v>614</v>
+      </c>
+      <c r="RM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RN2" t="s">
+        <v>556</v>
+      </c>
+      <c r="RO2" t="s">
+        <v>558</v>
+      </c>
+      <c r="RP2" t="s">
+        <v>557</v>
+      </c>
+      <c r="RQ2" t="s">
+        <v>558</v>
+      </c>
+      <c r="RR2" t="s">
+        <v>556</v>
+      </c>
+      <c r="RS2" t="s">
+        <v>558</v>
+      </c>
+      <c r="RT2" t="s">
+        <v>630</v>
+      </c>
+      <c r="RU2" t="s">
+        <v>563</v>
+      </c>
+      <c r="RV2" t="s">
+        <v>629</v>
+      </c>
+      <c r="RW2" t="s">
+        <v>593</v>
+      </c>
+      <c r="RX2" t="s">
+        <v>564</v>
+      </c>
+      <c r="RY2" t="s">
+        <v>565</v>
+      </c>
+      <c r="RZ2" t="s">
+        <v>538</v>
+      </c>
+      <c r="SA2" t="s">
+        <v>534</v>
+      </c>
+      <c r="SB2" t="s">
+        <v>566</v>
+      </c>
+      <c r="SC2" t="s">
+        <v>567</v>
+      </c>
+      <c r="SD2" t="s">
+        <v>568</v>
+      </c>
+      <c r="SE2" t="s">
+        <v>556</v>
+      </c>
+      <c r="SF2" t="s">
+        <v>534</v>
+      </c>
+      <c r="SG2" t="s">
+        <v>566</v>
+      </c>
+      <c r="SH2" t="s">
+        <v>569</v>
+      </c>
+      <c r="SI2" t="s">
+        <v>570</v>
+      </c>
+      <c r="SJ2" t="s">
+        <v>550</v>
+      </c>
+      <c r="SK2" t="s">
+        <v>534</v>
+      </c>
+      <c r="SL2" t="s">
+        <v>566</v>
+      </c>
+      <c r="SM2" t="s">
+        <v>571</v>
+      </c>
+      <c r="SN2" t="s">
+        <v>538</v>
+      </c>
+      <c r="SO2" t="s">
+        <v>572</v>
+      </c>
+      <c r="SP2" t="s">
+        <v>573</v>
+      </c>
+      <c r="SQ2" t="s">
+        <v>574</v>
+      </c>
+      <c r="SR2" t="s">
         <v>554</v>
       </c>
-      <c r="HX2" t="s">
-        <v>555</v>
-      </c>
-      <c r="HY2" t="s">
-        <v>544</v>
-      </c>
-      <c r="HZ2" t="s">
-        <v>522</v>
-      </c>
-      <c r="IA2" t="s">
-        <v>553</v>
-      </c>
-      <c r="IB2" t="s">
+      <c r="SS2" t="s">
+        <v>524</v>
+      </c>
+      <c r="ST2" t="s">
+        <v>575</v>
+      </c>
+      <c r="SU2" t="s">
+        <v>576</v>
+      </c>
+      <c r="SV2" t="s">
+        <v>577</v>
+      </c>
+      <c r="SW2" t="s">
+        <v>578</v>
+      </c>
+      <c r="SX2" t="s">
+        <v>579</v>
+      </c>
+      <c r="SY2" t="s">
+        <v>580</v>
+      </c>
+      <c r="SZ2" t="s">
+        <v>581</v>
+      </c>
+      <c r="TA2" t="s">
+        <v>582</v>
+      </c>
+      <c r="TB2" t="s">
+        <v>583</v>
+      </c>
+      <c r="TC2" t="s">
+        <v>558</v>
+      </c>
+      <c r="TD2" t="s">
+        <v>584</v>
+      </c>
+      <c r="TE2" t="s">
+        <v>585</v>
+      </c>
+      <c r="TF2" t="s">
+        <v>586</v>
+      </c>
+      <c r="TG2" t="s">
+        <v>583</v>
+      </c>
+      <c r="TH2" t="s">
+        <v>587</v>
+      </c>
+      <c r="TI2" t="s">
+        <v>588</v>
+      </c>
+      <c r="TJ2" t="s">
+        <v>589</v>
+      </c>
+      <c r="TK2" t="s">
+        <v>590</v>
+      </c>
+      <c r="TL2" t="s">
         <v>556</v>
       </c>
-      <c r="IC2" t="s">
-        <v>557</v>
-      </c>
-      <c r="ID2" t="s">
+      <c r="TM2" t="s">
         <v>538</v>
       </c>
-      <c r="IE2" t="s">
-        <v>522</v>
-      </c>
-      <c r="IF2" t="s">
-        <v>553</v>
-      </c>
-      <c r="IG2" t="s">
+      <c r="TN2" t="s">
+        <v>568</v>
+      </c>
+      <c r="TO2" t="s">
+        <v>591</v>
+      </c>
+      <c r="TP2" t="s">
+        <v>614</v>
+      </c>
+      <c r="TQ2" t="s">
+        <v>563</v>
+      </c>
+      <c r="TR2" t="s">
+        <v>587</v>
+      </c>
+      <c r="TS2" t="s">
         <v>558</v>
       </c>
-      <c r="IH2" t="s">
-        <v>526</v>
-      </c>
-      <c r="II2" t="s">
+      <c r="TT2" t="s">
+        <v>529</v>
+      </c>
+      <c r="TU2" t="s">
+        <v>631</v>
+      </c>
+      <c r="TV2" t="s">
         <v>559</v>
       </c>
-      <c r="IJ2" t="s">
-        <v>560</v>
-      </c>
-      <c r="IK2" t="s">
+      <c r="TW2" t="s">
+        <v>538</v>
+      </c>
+      <c r="TX2" t="s">
+        <v>632</v>
+      </c>
+      <c r="TY2" t="s">
+        <v>632</v>
+      </c>
+      <c r="TZ2" t="s">
+        <v>597</v>
+      </c>
+      <c r="UA2" t="s">
+        <v>534</v>
+      </c>
+      <c r="UB2" t="s">
+        <v>598</v>
+      </c>
+      <c r="UC2" t="s">
+        <v>534</v>
+      </c>
+      <c r="UD2" t="s">
+        <v>598</v>
+      </c>
+      <c r="UE2" t="s">
+        <v>534</v>
+      </c>
+      <c r="UF2" t="s">
+        <v>598</v>
+      </c>
+      <c r="UG2" t="s">
+        <v>529</v>
+      </c>
+      <c r="UH2" t="s">
+        <v>632</v>
+      </c>
+      <c r="UI2" t="s">
+        <v>632</v>
+      </c>
+      <c r="UJ2" t="s">
+        <v>597</v>
+      </c>
+      <c r="UK2" t="s">
+        <v>534</v>
+      </c>
+      <c r="UL2" t="s">
+        <v>598</v>
+      </c>
+      <c r="UM2" t="s">
+        <v>534</v>
+      </c>
+      <c r="UN2" t="s">
+        <v>598</v>
+      </c>
+      <c r="UO2" t="s">
+        <v>534</v>
+      </c>
+      <c r="UP2" t="s">
+        <v>598</v>
+      </c>
+      <c r="UQ2" t="s">
+        <v>633</v>
+      </c>
+      <c r="UR2" t="s">
+        <v>598</v>
+      </c>
+      <c r="US2" t="s">
+        <v>606</v>
+      </c>
+      <c r="UT2" t="s">
+        <v>605</v>
+      </c>
+      <c r="UU2" t="s">
+        <v>556</v>
+      </c>
+      <c r="UV2" t="s">
+        <v>556</v>
+      </c>
+      <c r="UW2" t="s">
+        <v>634</v>
+      </c>
+      <c r="UX2" t="s">
+        <v>529</v>
+      </c>
+      <c r="UY2" t="s">
+        <v>550</v>
+      </c>
+      <c r="UZ2" t="s">
+        <v>602</v>
+      </c>
+      <c r="VA2" t="s">
+        <v>635</v>
+      </c>
+      <c r="VB2" t="s">
+        <v>529</v>
+      </c>
+      <c r="VC2" t="s">
+        <v>593</v>
+      </c>
+      <c r="VD2" t="s">
+        <v>556</v>
+      </c>
+      <c r="VE2" t="s">
+        <v>636</v>
+      </c>
+      <c r="VF2" t="s">
+        <v>605</v>
+      </c>
+      <c r="VG2" t="s">
+        <v>550</v>
+      </c>
+      <c r="VH2" t="s">
+        <v>524</v>
+      </c>
+      <c r="VI2" t="s">
+        <v>602</v>
+      </c>
+      <c r="VJ2" t="s">
+        <v>524</v>
+      </c>
+      <c r="VK2" t="s">
+        <v>566</v>
+      </c>
+      <c r="VL2" t="s">
         <v>561</v>
       </c>
-      <c r="IL2" t="s">
-        <v>542</v>
-      </c>
-      <c r="IM2" t="s">
-        <v>562</v>
-      </c>
-      <c r="IN2" t="s">
-        <v>563</v>
-      </c>
-      <c r="IO2" t="s">
-        <v>564</v>
-      </c>
-      <c r="IP2" t="s">
-        <v>565</v>
-      </c>
-      <c r="IQ2" t="s">
+      <c r="VM2" t="s">
+        <v>559</v>
+      </c>
+      <c r="VN2" t="s">
+        <v>550</v>
+      </c>
+      <c r="VO2" t="s">
+        <v>637</v>
+      </c>
+      <c r="VP2" t="s">
+        <v>637</v>
+      </c>
+      <c r="VQ2" t="s">
+        <v>637</v>
+      </c>
+      <c r="VR2" t="s">
+        <v>637</v>
+      </c>
+      <c r="VS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="VT2" t="s">
+        <v>558</v>
+      </c>
+      <c r="VU2" t="s">
+        <v>583</v>
+      </c>
+      <c r="VV2" t="s">
+        <v>638</v>
+      </c>
+      <c r="VW2" t="s">
+        <v>609</v>
+      </c>
+      <c r="VX2" t="s">
+        <v>639</v>
+      </c>
+      <c r="VY2" t="s">
+        <v>640</v>
+      </c>
+      <c r="VZ2" t="s">
+        <v>559</v>
+      </c>
+      <c r="WA2" t="s">
+        <v>593</v>
+      </c>
+      <c r="WB2" t="s">
+        <v>641</v>
+      </c>
+      <c r="WC2" t="s">
+        <v>626</v>
+      </c>
+      <c r="WD2" t="s">
+        <v>608</v>
+      </c>
+      <c r="WE2" t="s">
+        <v>601</v>
+      </c>
+      <c r="WF2" t="s">
+        <v>642</v>
+      </c>
+      <c r="WG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="WH2" t="s">
+        <v>559</v>
+      </c>
+      <c r="WI2" t="s">
+        <v>534</v>
+      </c>
+      <c r="WJ2" t="s">
         <v>566</v>
       </c>
-      <c r="IR2" t="s">
-        <v>567</v>
-      </c>
-      <c r="IS2" t="s">
-        <v>568</v>
-      </c>
-      <c r="IT2" t="s">
-        <v>569</v>
-      </c>
-      <c r="IU2" t="s">
-        <v>570</v>
-      </c>
-      <c r="IV2" t="s">
-        <v>571</v>
-      </c>
-      <c r="IW2" t="s">
-        <v>546</v>
-      </c>
-      <c r="IX2" t="s">
-        <v>572</v>
-      </c>
-      <c r="IY2" t="s">
-        <v>573</v>
-      </c>
-      <c r="IZ2" t="s">
-        <v>574</v>
-      </c>
-      <c r="JA2" t="s">
-        <v>571</v>
-      </c>
-      <c r="JB2" t="s">
-        <v>575</v>
-      </c>
-      <c r="JC2" t="s">
-        <v>576</v>
-      </c>
-      <c r="JD2" t="s">
-        <v>577</v>
-      </c>
-      <c r="JE2" t="s">
-        <v>578</v>
-      </c>
-      <c r="JF2" t="s">
-        <v>544</v>
-      </c>
-      <c r="JG2" t="s">
-        <v>526</v>
-      </c>
-      <c r="JH2" t="s">
-        <v>555</v>
-      </c>
-      <c r="JI2" t="s">
-        <v>579</v>
-      </c>
-      <c r="JJ2" t="s">
-        <v>580</v>
-      </c>
-      <c r="JK2" t="s">
-        <v>581</v>
-      </c>
-      <c r="JL2" t="s">
-        <v>582</v>
-      </c>
-      <c r="JM2" t="s">
-        <v>519</v>
-      </c>
-      <c r="JN2" t="s">
-        <v>522</v>
-      </c>
-      <c r="JO2" t="s">
-        <v>583</v>
-      </c>
-      <c r="JP2" t="s">
-        <v>584</v>
-      </c>
-      <c r="JQ2" t="s">
-        <v>562</v>
-      </c>
-      <c r="JR2" t="s">
-        <v>585</v>
-      </c>
-      <c r="JS2" t="s">
-        <v>585</v>
-      </c>
-      <c r="JT2" t="s">
-        <v>586</v>
-      </c>
-      <c r="JU2" t="s">
-        <v>522</v>
-      </c>
-      <c r="JV2" t="s">
-        <v>586</v>
-      </c>
-      <c r="JW2" t="s">
-        <v>522</v>
-      </c>
-      <c r="JX2" t="s">
-        <v>586</v>
-      </c>
-      <c r="JY2" t="s">
-        <v>522</v>
-      </c>
-      <c r="JZ2" t="s">
-        <v>586</v>
-      </c>
-      <c r="KA2" t="s">
-        <v>512</v>
-      </c>
-      <c r="KB2" t="s">
-        <v>585</v>
-      </c>
-      <c r="KC2" t="s">
-        <v>585</v>
-      </c>
-      <c r="KD2" t="s">
-        <v>586</v>
-      </c>
-      <c r="KE2" t="s">
-        <v>522</v>
-      </c>
-      <c r="KF2" t="s">
-        <v>586</v>
-      </c>
-      <c r="KG2" t="s">
-        <v>522</v>
-      </c>
-      <c r="KH2" t="s">
-        <v>586</v>
-      </c>
-      <c r="KI2" t="s">
-        <v>522</v>
-      </c>
-      <c r="KJ2" t="s">
-        <v>586</v>
-      </c>
-      <c r="KK2" t="s">
-        <v>587</v>
-      </c>
-      <c r="KL2" t="s">
-        <v>586</v>
-      </c>
-      <c r="KM2" t="s">
-        <v>588</v>
-      </c>
-      <c r="KN2" t="s">
-        <v>526</v>
-      </c>
-      <c r="KO2" t="s">
-        <v>589</v>
-      </c>
-      <c r="KP2" t="s">
-        <v>590</v>
-      </c>
-      <c r="KQ2" t="s">
-        <v>591</v>
-      </c>
-      <c r="KR2" t="s">
-        <v>517</v>
-      </c>
-      <c r="KS2" t="s">
-        <v>544</v>
-      </c>
-      <c r="KT2" t="s">
-        <v>544</v>
-      </c>
-      <c r="KU2" t="s">
-        <v>592</v>
-      </c>
-      <c r="KV2" t="s">
-        <v>593</v>
-      </c>
-      <c r="KW2" t="s">
-        <v>538</v>
-      </c>
-      <c r="KX2" t="s">
-        <v>562</v>
-      </c>
-      <c r="KY2" t="s">
-        <v>594</v>
-      </c>
-      <c r="KZ2" t="s">
-        <v>512</v>
-      </c>
-      <c r="LA2" t="s">
-        <v>581</v>
-      </c>
-      <c r="LB2" t="s">
-        <v>562</v>
-      </c>
-      <c r="LC2" t="s">
-        <v>544</v>
-      </c>
-      <c r="LD2" t="s">
-        <v>517</v>
-      </c>
-      <c r="LE2" t="s">
-        <v>546</v>
-      </c>
-      <c r="LF2" t="s">
-        <v>546</v>
-      </c>
-      <c r="LG2" t="s">
-        <v>538</v>
-      </c>
-      <c r="LH2" t="s">
-        <v>553</v>
-      </c>
-      <c r="LI2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LJ2" t="s">
-        <v>538</v>
-      </c>
-      <c r="LK2" t="s">
-        <v>542</v>
-      </c>
-      <c r="LL2" t="s">
-        <v>595</v>
-      </c>
-      <c r="LM2" t="s">
-        <v>596</v>
-      </c>
-      <c r="LN2" t="s">
-        <v>597</v>
-      </c>
-      <c r="LO2" t="s">
-        <v>598</v>
-      </c>
-      <c r="LP2" t="s">
-        <v>599</v>
-      </c>
-      <c r="LQ2" t="s">
-        <v>538</v>
-      </c>
-      <c r="LR2" t="s">
-        <v>558</v>
-      </c>
-      <c r="LS2" t="s">
-        <v>600</v>
-      </c>
-      <c r="LT2" t="s">
-        <v>601</v>
-      </c>
-      <c r="LU2" t="s">
-        <v>542</v>
-      </c>
-      <c r="LV2" t="s">
-        <v>602</v>
-      </c>
-      <c r="LW2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LX2" t="s">
-        <v>582</v>
-      </c>
-      <c r="LY2" t="s">
-        <v>593</v>
-      </c>
-      <c r="LZ2" t="s">
-        <v>553</v>
-      </c>
-      <c r="MA2" t="s">
-        <v>519</v>
-      </c>
-      <c r="MB2" t="s">
-        <v>603</v>
-      </c>
-      <c r="MC2" t="s">
-        <v>558</v>
-      </c>
-      <c r="MD2" t="s">
-        <v>604</v>
-      </c>
-      <c r="ME2" t="s">
-        <v>542</v>
-      </c>
-      <c r="MF2" t="s">
-        <v>137</v>
-      </c>
-      <c r="MG2" t="s">
-        <v>517</v>
-      </c>
-      <c r="MH2" t="s">
-        <v>562</v>
-      </c>
-      <c r="MI2" t="s">
-        <v>605</v>
-      </c>
-      <c r="MJ2" t="s">
-        <v>512</v>
-      </c>
-      <c r="MK2" t="s">
-        <v>517</v>
-      </c>
-      <c r="ML2" t="s">
-        <v>512</v>
-      </c>
-      <c r="MM2" t="s">
-        <v>547</v>
-      </c>
-      <c r="MN2" t="s">
-        <v>548</v>
-      </c>
-      <c r="MO2" t="s">
-        <v>598</v>
-      </c>
-      <c r="MP2" t="s">
-        <v>546</v>
-      </c>
-      <c r="MQ2" t="s">
-        <v>551</v>
-      </c>
-      <c r="MR2" t="s">
-        <v>552</v>
-      </c>
-      <c r="MS2" t="s">
-        <v>526</v>
-      </c>
-      <c r="MT2" t="s">
-        <v>522</v>
-      </c>
-      <c r="MU2" t="s">
-        <v>553</v>
-      </c>
-      <c r="MV2" t="s">
+      <c r="WK2" t="s">
+        <v>524</v>
+      </c>
+      <c r="WL2" t="s">
+        <v>643</v>
+      </c>
+      <c r="WM2" t="s">
         <v>554</v>
       </c>
-      <c r="MW2" t="s">
-        <v>555</v>
-      </c>
-      <c r="MX2" t="s">
-        <v>544</v>
-      </c>
-      <c r="MY2" t="s">
-        <v>522</v>
-      </c>
-      <c r="MZ2" t="s">
-        <v>553</v>
-      </c>
-      <c r="NA2" t="s">
-        <v>556</v>
-      </c>
-      <c r="NB2" t="s">
-        <v>557</v>
-      </c>
-      <c r="NC2" t="s">
-        <v>538</v>
-      </c>
-      <c r="ND2" t="s">
-        <v>522</v>
-      </c>
-      <c r="NE2" t="s">
-        <v>553</v>
-      </c>
-      <c r="NF2" t="s">
-        <v>558</v>
-      </c>
-      <c r="NG2" t="s">
-        <v>526</v>
-      </c>
-      <c r="NH2" t="s">
-        <v>559</v>
-      </c>
-      <c r="NI2" t="s">
-        <v>560</v>
-      </c>
-      <c r="NJ2" t="s">
-        <v>561</v>
-      </c>
-      <c r="NK2" t="s">
-        <v>542</v>
-      </c>
-      <c r="NL2" t="s">
-        <v>562</v>
-      </c>
-      <c r="NM2" t="s">
-        <v>563</v>
-      </c>
-      <c r="NN2" t="s">
-        <v>564</v>
-      </c>
-      <c r="NO2" t="s">
-        <v>565</v>
-      </c>
-      <c r="NP2" t="s">
-        <v>566</v>
-      </c>
-      <c r="NQ2" t="s">
-        <v>567</v>
-      </c>
-      <c r="NR2" t="s">
-        <v>568</v>
-      </c>
-      <c r="NS2" t="s">
-        <v>569</v>
-      </c>
-      <c r="NT2" t="s">
-        <v>570</v>
-      </c>
-      <c r="NU2" t="s">
-        <v>571</v>
-      </c>
-      <c r="NV2" t="s">
-        <v>546</v>
-      </c>
-      <c r="NW2" t="s">
-        <v>572</v>
-      </c>
-      <c r="NX2" t="s">
-        <v>573</v>
-      </c>
-      <c r="NY2" t="s">
-        <v>574</v>
-      </c>
-      <c r="NZ2" t="s">
-        <v>571</v>
-      </c>
-      <c r="OA2" t="s">
-        <v>575</v>
-      </c>
-      <c r="OB2" t="s">
-        <v>576</v>
-      </c>
-      <c r="OC2" t="s">
-        <v>577</v>
-      </c>
-      <c r="OD2" t="s">
-        <v>578</v>
-      </c>
-      <c r="OE2" t="s">
-        <v>544</v>
-      </c>
-      <c r="OF2" t="s">
-        <v>526</v>
-      </c>
-      <c r="OG2" t="s">
-        <v>555</v>
-      </c>
-      <c r="OH2" t="s">
-        <v>579</v>
-      </c>
-      <c r="OI2" t="s">
-        <v>598</v>
-      </c>
-      <c r="OJ2" t="s">
-        <v>606</v>
-      </c>
-      <c r="OK2" t="s">
-        <v>582</v>
-      </c>
-      <c r="OL2" t="s">
-        <v>546</v>
-      </c>
-      <c r="OM2" t="s">
-        <v>512</v>
-      </c>
-      <c r="ON2" t="s">
-        <v>605</v>
-      </c>
-      <c r="OO2" t="s">
-        <v>538</v>
-      </c>
-      <c r="OP2" t="s">
-        <v>517</v>
-      </c>
-      <c r="OQ2" t="s">
-        <v>585</v>
-      </c>
-      <c r="OR2" t="s">
-        <v>585</v>
-      </c>
-      <c r="OS2" t="s">
-        <v>586</v>
-      </c>
-      <c r="OT2" t="s">
-        <v>522</v>
-      </c>
-      <c r="OU2" t="s">
-        <v>586</v>
-      </c>
-      <c r="OV2" t="s">
-        <v>522</v>
-      </c>
-      <c r="OW2" t="s">
-        <v>586</v>
-      </c>
-      <c r="OX2" t="s">
-        <v>522</v>
-      </c>
-      <c r="OY2" t="s">
-        <v>586</v>
-      </c>
-      <c r="OZ2" t="s">
-        <v>590</v>
-      </c>
-      <c r="PA2" t="s">
-        <v>585</v>
-      </c>
-      <c r="PB2" t="s">
-        <v>585</v>
-      </c>
-      <c r="PC2" t="s">
-        <v>586</v>
-      </c>
-      <c r="PD2" t="s">
-        <v>522</v>
-      </c>
-      <c r="PE2" t="s">
-        <v>586</v>
-      </c>
-      <c r="PF2" t="s">
-        <v>522</v>
-      </c>
-      <c r="PG2" t="s">
-        <v>586</v>
-      </c>
-      <c r="PH2" t="s">
-        <v>522</v>
-      </c>
-      <c r="PI2" t="s">
-        <v>586</v>
-      </c>
-      <c r="PJ2" t="s">
-        <v>607</v>
-      </c>
-      <c r="PK2" t="s">
-        <v>586</v>
-      </c>
-      <c r="PL2" t="s">
-        <v>608</v>
-      </c>
-      <c r="PM2" t="s">
-        <v>590</v>
-      </c>
-      <c r="PN2" t="s">
-        <v>544</v>
-      </c>
-      <c r="PO2" t="s">
-        <v>517</v>
-      </c>
-      <c r="PP2" t="s">
-        <v>609</v>
-      </c>
-      <c r="PQ2" t="s">
-        <v>544</v>
-      </c>
-      <c r="PR2" t="s">
-        <v>562</v>
-      </c>
-      <c r="PS2" t="s">
-        <v>593</v>
-      </c>
-      <c r="PT2" t="s">
-        <v>610</v>
-      </c>
-      <c r="PU2" t="s">
-        <v>544</v>
-      </c>
-      <c r="PV2" t="s">
-        <v>548</v>
-      </c>
-      <c r="PW2" t="s">
-        <v>517</v>
-      </c>
-      <c r="PX2" t="s">
-        <v>611</v>
-      </c>
-      <c r="PY2" t="s">
-        <v>590</v>
-      </c>
-      <c r="PZ2" t="s">
-        <v>538</v>
-      </c>
-      <c r="QA2" t="s">
-        <v>517</v>
-      </c>
-      <c r="QB2" t="s">
-        <v>593</v>
-      </c>
-      <c r="QC2" t="s">
-        <v>526</v>
-      </c>
-      <c r="QD2" t="s">
-        <v>546</v>
-      </c>
-      <c r="QE2" t="s">
-        <v>546</v>
-      </c>
-      <c r="QF2" t="s">
-        <v>562</v>
-      </c>
-      <c r="QG2" t="s">
-        <v>519</v>
-      </c>
-      <c r="QH2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QI2" t="s">
-        <v>538</v>
-      </c>
-      <c r="QJ2" t="s">
-        <v>571</v>
-      </c>
-      <c r="QK2" t="s">
-        <v>595</v>
-      </c>
-      <c r="QL2" t="s">
-        <v>596</v>
-      </c>
-      <c r="QM2" t="s">
-        <v>597</v>
-      </c>
-      <c r="QN2" t="s">
-        <v>612</v>
-      </c>
-      <c r="QO2" t="s">
-        <v>512</v>
-      </c>
-      <c r="QP2" t="s">
-        <v>512</v>
-      </c>
-      <c r="QQ2" t="s">
-        <v>558</v>
-      </c>
-      <c r="QR2" t="s">
-        <v>598</v>
-      </c>
-      <c r="QS2" t="s">
-        <v>595</v>
-      </c>
-      <c r="QT2" t="s">
-        <v>589</v>
-      </c>
-      <c r="QU2" t="s">
+      <c r="WN2" t="s">
         <v>613</v>
       </c>
-      <c r="QV2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QW2" t="s">
-        <v>582</v>
-      </c>
-      <c r="QX2" t="s">
-        <v>522</v>
-      </c>
-      <c r="QY2" t="s">
-        <v>593</v>
-      </c>
-      <c r="QZ2" t="s">
-        <v>546</v>
-      </c>
-      <c r="RA2" t="s">
-        <v>614</v>
-      </c>
-      <c r="RB2" t="s">
-        <v>615</v>
-      </c>
-      <c r="RC2" t="s">
-        <v>571</v>
-      </c>
-      <c r="RD2" t="s">
-        <v>601</v>
-      </c>
-      <c r="RE2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RF2" t="s">
-        <v>544</v>
-      </c>
-      <c r="RG2" t="s">
-        <v>546</v>
-      </c>
-      <c r="RH2" t="s">
-        <v>545</v>
-      </c>
-      <c r="RI2" t="s">
-        <v>546</v>
-      </c>
-      <c r="RJ2" t="s">
-        <v>544</v>
-      </c>
-      <c r="RK2" t="s">
-        <v>546</v>
-      </c>
-      <c r="RL2" t="s">
-        <v>616</v>
-      </c>
-      <c r="RM2" t="s">
-        <v>550</v>
-      </c>
-      <c r="RN2" t="s">
-        <v>615</v>
-      </c>
-      <c r="RO2" t="s">
-        <v>581</v>
-      </c>
-      <c r="RP2" t="s">
-        <v>551</v>
-      </c>
-      <c r="RQ2" t="s">
-        <v>552</v>
-      </c>
-      <c r="RR2" t="s">
-        <v>526</v>
-      </c>
-      <c r="RS2" t="s">
-        <v>522</v>
-      </c>
-      <c r="RT2" t="s">
-        <v>553</v>
-      </c>
-      <c r="RU2" t="s">
-        <v>554</v>
-      </c>
-      <c r="RV2" t="s">
-        <v>555</v>
-      </c>
-      <c r="RW2" t="s">
-        <v>544</v>
-      </c>
-      <c r="RX2" t="s">
-        <v>522</v>
-      </c>
-      <c r="RY2" t="s">
-        <v>553</v>
-      </c>
-      <c r="RZ2" t="s">
-        <v>556</v>
-      </c>
-      <c r="SA2" t="s">
-        <v>557</v>
-      </c>
-      <c r="SB2" t="s">
-        <v>538</v>
-      </c>
-      <c r="SC2" t="s">
-        <v>522</v>
-      </c>
-      <c r="SD2" t="s">
-        <v>553</v>
-      </c>
-      <c r="SE2" t="s">
-        <v>558</v>
-      </c>
-      <c r="SF2" t="s">
-        <v>526</v>
-      </c>
-      <c r="SG2" t="s">
-        <v>559</v>
-      </c>
-      <c r="SH2" t="s">
-        <v>560</v>
-      </c>
-      <c r="SI2" t="s">
-        <v>561</v>
-      </c>
-      <c r="SJ2" t="s">
-        <v>542</v>
-      </c>
-      <c r="SK2" t="s">
-        <v>562</v>
-      </c>
-      <c r="SL2" t="s">
-        <v>563</v>
-      </c>
-      <c r="SM2" t="s">
-        <v>564</v>
-      </c>
-      <c r="SN2" t="s">
-        <v>565</v>
-      </c>
-      <c r="SO2" t="s">
-        <v>566</v>
-      </c>
-      <c r="SP2" t="s">
-        <v>567</v>
-      </c>
-      <c r="SQ2" t="s">
-        <v>568</v>
-      </c>
-      <c r="SR2" t="s">
-        <v>569</v>
-      </c>
-      <c r="SS2" t="s">
-        <v>570</v>
-      </c>
-      <c r="ST2" t="s">
-        <v>571</v>
-      </c>
-      <c r="SU2" t="s">
-        <v>546</v>
-      </c>
-      <c r="SV2" t="s">
-        <v>572</v>
-      </c>
-      <c r="SW2" t="s">
-        <v>573</v>
-      </c>
-      <c r="SX2" t="s">
-        <v>574</v>
-      </c>
-      <c r="SY2" t="s">
-        <v>571</v>
-      </c>
-      <c r="SZ2" t="s">
-        <v>575</v>
-      </c>
-      <c r="TA2" t="s">
-        <v>576</v>
-      </c>
-      <c r="TB2" t="s">
-        <v>577</v>
-      </c>
-      <c r="TC2" t="s">
-        <v>578</v>
-      </c>
-      <c r="TD2" t="s">
-        <v>544</v>
-      </c>
-      <c r="TE2" t="s">
-        <v>526</v>
-      </c>
-      <c r="TF2" t="s">
-        <v>555</v>
-      </c>
-      <c r="TG2" t="s">
-        <v>579</v>
-      </c>
-      <c r="TH2" t="s">
-        <v>601</v>
-      </c>
-      <c r="TI2" t="s">
-        <v>550</v>
-      </c>
-      <c r="TJ2" t="s">
-        <v>575</v>
-      </c>
-      <c r="TK2" t="s">
-        <v>546</v>
-      </c>
-      <c r="TL2" t="s">
-        <v>517</v>
-      </c>
-      <c r="TM2" t="s">
-        <v>617</v>
-      </c>
-      <c r="TN2" t="s">
-        <v>512</v>
-      </c>
-      <c r="TO2" t="s">
-        <v>526</v>
-      </c>
-      <c r="TP2" t="s">
-        <v>618</v>
-      </c>
-      <c r="TQ2" t="s">
-        <v>618</v>
-      </c>
-      <c r="TR2" t="s">
-        <v>585</v>
-      </c>
-      <c r="TS2" t="s">
-        <v>522</v>
-      </c>
-      <c r="TT2" t="s">
-        <v>586</v>
-      </c>
-      <c r="TU2" t="s">
-        <v>522</v>
-      </c>
-      <c r="TV2" t="s">
-        <v>586</v>
-      </c>
-      <c r="TW2" t="s">
-        <v>522</v>
-      </c>
-      <c r="TX2" t="s">
-        <v>586</v>
-      </c>
-      <c r="TY2" t="s">
-        <v>517</v>
-      </c>
-      <c r="TZ2" t="s">
-        <v>618</v>
-      </c>
-      <c r="UA2" t="s">
-        <v>618</v>
-      </c>
-      <c r="UB2" t="s">
-        <v>585</v>
-      </c>
-      <c r="UC2" t="s">
-        <v>522</v>
-      </c>
-      <c r="UD2" t="s">
-        <v>586</v>
-      </c>
-      <c r="UE2" t="s">
-        <v>522</v>
-      </c>
-      <c r="UF2" t="s">
-        <v>586</v>
-      </c>
-      <c r="UG2" t="s">
-        <v>522</v>
-      </c>
-      <c r="UH2" t="s">
-        <v>586</v>
-      </c>
-      <c r="UI2" t="s">
-        <v>619</v>
-      </c>
-      <c r="UJ2" t="s">
-        <v>586</v>
-      </c>
-      <c r="UK2" t="s">
-        <v>594</v>
-      </c>
-      <c r="UL2" t="s">
-        <v>593</v>
-      </c>
-      <c r="UM2" t="s">
-        <v>544</v>
-      </c>
-      <c r="UN2" t="s">
-        <v>544</v>
-      </c>
-      <c r="UO2" t="s">
-        <v>620</v>
-      </c>
-      <c r="UP2" t="s">
-        <v>517</v>
-      </c>
-      <c r="UQ2" t="s">
-        <v>538</v>
-      </c>
-      <c r="UR2" t="s">
-        <v>590</v>
-      </c>
-      <c r="US2" t="s">
-        <v>621</v>
-      </c>
-      <c r="UT2" t="s">
-        <v>517</v>
-      </c>
-      <c r="UU2" t="s">
-        <v>581</v>
-      </c>
-      <c r="UV2" t="s">
-        <v>544</v>
-      </c>
-      <c r="UW2" t="s">
-        <v>622</v>
-      </c>
-      <c r="UX2" t="s">
-        <v>593</v>
-      </c>
-      <c r="UY2" t="s">
-        <v>538</v>
-      </c>
-      <c r="UZ2" t="s">
-        <v>562</v>
-      </c>
-      <c r="VA2" t="s">
-        <v>590</v>
-      </c>
-      <c r="VB2" t="s">
-        <v>562</v>
-      </c>
-      <c r="VC2" t="s">
-        <v>553</v>
-      </c>
-      <c r="VD2" t="s">
-        <v>548</v>
-      </c>
-      <c r="VE2" t="s">
-        <v>512</v>
-      </c>
-      <c r="VF2" t="s">
-        <v>538</v>
-      </c>
-      <c r="VG2" t="s">
-        <v>137</v>
-      </c>
-      <c r="VH2" t="s">
-        <v>546</v>
-      </c>
-      <c r="VI2" t="s">
-        <v>571</v>
-      </c>
-      <c r="VJ2" t="s">
-        <v>623</v>
-      </c>
-      <c r="VK2" t="s">
-        <v>596</v>
-      </c>
-      <c r="VL2" t="s">
-        <v>624</v>
-      </c>
-      <c r="VM2" t="s">
-        <v>625</v>
-      </c>
-      <c r="VN2" t="s">
-        <v>512</v>
-      </c>
-      <c r="VO2" t="s">
-        <v>581</v>
-      </c>
-      <c r="VP2" t="s">
+      <c r="WO2" t="s">
         <v>626</v>
-      </c>
-      <c r="VQ2" t="s">
-        <v>612</v>
-      </c>
-      <c r="VR2" t="s">
-        <v>595</v>
-      </c>
-      <c r="VS2" t="s">
-        <v>589</v>
-      </c>
-      <c r="VT2" t="s">
-        <v>627</v>
-      </c>
-      <c r="VU2" t="s">
-        <v>137</v>
-      </c>
-      <c r="VV2" t="s">
-        <v>512</v>
-      </c>
-      <c r="VW2" t="s">
-        <v>522</v>
-      </c>
-      <c r="VX2" t="s">
-        <v>553</v>
-      </c>
-      <c r="VY2" t="s">
-        <v>562</v>
-      </c>
-      <c r="VZ2" t="s">
-        <v>628</v>
-      </c>
-      <c r="WA2" t="s">
-        <v>542</v>
-      </c>
-      <c r="WB2" t="s">
-        <v>600</v>
-      </c>
-      <c r="WC2" t="s">
-        <v>612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>